<commit_message>
Correção doc de evid. testes MHS-15
</commit_message>
<xml_diff>
--- a/Testes/Documento de Testes - MHS-15.xlsx
+++ b/Testes/Documento de Testes - MHS-15.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\OneDrive\Documentos\Meus Projetos\My Hair Salon\Testes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EC9B9AE-391E-488E-BAC7-FC8D51C6D602}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B666FD0-77EA-48A4-9943-5ED51922F19D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{60EB7970-8BE6-4BE5-9238-E82C81D98BC0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{60EB7970-8BE6-4BE5-9238-E82C81D98BC0}"/>
   </bookViews>
   <sheets>
     <sheet name="Informações Gerais" sheetId="1" r:id="rId1"/>
@@ -39,80 +39,8 @@
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata">
-  <metadataTypes count="1">
-    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLRICHVALUE" count="6">
-    <bk>
-      <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
-          <xlrd:rvb i="0"/>
-        </ext>
-      </extLst>
-    </bk>
-    <bk>
-      <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
-          <xlrd:rvb i="1"/>
-        </ext>
-      </extLst>
-    </bk>
-    <bk>
-      <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
-          <xlrd:rvb i="2"/>
-        </ext>
-      </extLst>
-    </bk>
-    <bk>
-      <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
-          <xlrd:rvb i="3"/>
-        </ext>
-      </extLst>
-    </bk>
-    <bk>
-      <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
-          <xlrd:rvb i="4"/>
-        </ext>
-      </extLst>
-    </bk>
-    <bk>
-      <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
-          <xlrd:rvb i="5"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <valueMetadata count="6">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-    <bk>
-      <rc t="1" v="1"/>
-    </bk>
-    <bk>
-      <rc t="1" v="2"/>
-    </bk>
-    <bk>
-      <rc t="1" v="3"/>
-    </bk>
-    <bk>
-      <rc t="1" v="4"/>
-    </bk>
-    <bk>
-      <rc t="1" v="5"/>
-    </bk>
-  </valueMetadata>
-</metadata>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="42">
   <si>
     <t>Projeto</t>
   </si>
@@ -175,9 +103,6 @@
   </si>
   <si>
     <t>Gabriella Xavier</t>
-  </si>
-  <si>
-    <t>https://projeto-sistema-cabeleireiro.vercel.app/esqueciMinhaSenha.html</t>
   </si>
   <si>
     <t>https://gabsxavier01-1738650621002.atlassian.net/browse/MHS-15</t>
@@ -332,14 +257,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -494,95 +419,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
-<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
-  <global>
-    <keyFlags>
-      <key name="_Self">
-        <flag name="ExcludeFromFile" value="1"/>
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_DisplayString">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Flags">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Format">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_SubLabel">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Attribution">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Icon">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Display">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_CanonicalPropertyNames">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_ClassificationId">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-    </keyFlags>
-  </global>
-</rvTypesInfo>
-</file>
-
-<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="6">
-  <rv s="0">
-    <v>0</v>
-    <v>5</v>
-  </rv>
-  <rv s="0">
-    <v>1</v>
-    <v>5</v>
-  </rv>
-  <rv s="0">
-    <v>2</v>
-    <v>5</v>
-  </rv>
-  <rv s="0">
-    <v>3</v>
-    <v>5</v>
-  </rv>
-  <rv s="0">
-    <v>4</v>
-    <v>5</v>
-  </rv>
-  <rv s="0">
-    <v>5</v>
-    <v>5</v>
-  </rv>
-</rvData>
-</file>
-
-<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
-<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
-  <s t="_localImage">
-    <k n="_rvRel:LocalImageIdentifier" t="i"/>
-    <k n="CalcOrigin" t="i"/>
-  </s>
-</rvStructures>
-</file>
-
-<file path=xl/richData/richValueRel.xml><?xml version="1.0" encoding="utf-8"?>
-<richValueRels xmlns="http://schemas.microsoft.com/office/spreadsheetml/2022/richvaluerel" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rel r:id="rId1"/>
-  <rel r:id="rId2"/>
-  <rel r:id="rId3"/>
-  <rel r:id="rId4"/>
-  <rel r:id="rId5"/>
-  <rel r:id="rId6"/>
-</richValueRels>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -904,8 +740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC0A0962-7C6C-4640-A9C3-D61D95AF0094}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -916,16 +752,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="7"/>
-      <c r="B1" s="7"/>
+      <c r="A1" s="9"/>
+      <c r="B1" s="9"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4"/>
@@ -943,7 +779,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -951,7 +787,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -982,9 +818,7 @@
       <c r="A11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>21</v>
-      </c>
+      <c r="B11" s="3"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
@@ -1007,8 +841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5E8ABBC-E64F-4728-8C3E-82E71C484C73}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView showGridLines="0" topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1020,37 +854,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="7"/>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
+      <c r="A1" s="9"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
@@ -1078,144 +912,132 @@
         <v>17</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="192.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>1</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="9" t="s">
+      <c r="E7" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="F7" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="H7" s="6" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
+      <c r="H7" s="6"/>
       <c r="I7" s="6"/>
     </row>
     <row r="8" spans="1:9" ht="192.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <v>2</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="9" t="s">
+      <c r="E8" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="F8" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="H8" s="6" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
+      <c r="G8" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" s="6"/>
       <c r="I8" s="6"/>
     </row>
     <row r="9" spans="1:9" ht="192.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <v>3</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="9" t="s">
+      <c r="B9" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="F9" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="H9" s="6" t="e" vm="3">
-        <v>#VALUE!</v>
-      </c>
-      <c r="I9" s="6" t="e" vm="4">
-        <v>#VALUE!</v>
-      </c>
+      <c r="G9" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
     </row>
     <row r="10" spans="1:9" ht="192.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <v>4</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10" s="9" t="s">
+      <c r="F10" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="F10" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="H10" s="6" t="e" vm="5">
-        <v>#VALUE!</v>
-      </c>
+      <c r="G10" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10" s="6"/>
       <c r="I10" s="6"/>
     </row>
     <row r="11" spans="1:9" ht="192.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <v>5</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" s="9" t="s">
+      <c r="F11" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="F11" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="H11" s="6" t="e" vm="6">
-        <v>#VALUE!</v>
-      </c>
+      <c r="G11" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H11" s="6"/>
       <c r="I11" s="6"/>
     </row>
   </sheetData>

</xml_diff>